<commit_message>
Added SQL query for inserting into staging tables
</commit_message>
<xml_diff>
--- a/testdata/CBO-Smoke-TestData.xlsx
+++ b/testdata/CBO-Smoke-TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Srividhya\Playwright - discovery handson\CBO - Smoke\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575D83EC-033B-4143-A67D-3DAF582DBED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3962DAE9-08B8-474A-9C46-B0268ECDB2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -268,12 +268,6 @@
     <t>TC01_CBO_2under30</t>
   </si>
   <si>
-    <t>CBOSMOKEFN_$getcurrentdate</t>
-  </si>
-  <si>
-    <t>CBOSMOKELN_$getcurrentdate</t>
-  </si>
-  <si>
     <t>$GetContractID</t>
   </si>
   <si>
@@ -293,6 +287,18 @@
   </si>
   <si>
     <t>$GetCurrentDateMinus35</t>
+  </si>
+  <si>
+    <t>$GetContractSerialCollateralId</t>
+  </si>
+  <si>
+    <t>$GetFirstName</t>
+  </si>
+  <si>
+    <t>$GetLastName</t>
+  </si>
+  <si>
+    <t>01/01/1989</t>
   </si>
 </sst>
 </file>
@@ -746,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E450987-3812-44CB-89CB-24F32111945A}">
   <dimension ref="A1:BR8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,16 +984,16 @@
         <v>79</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
@@ -996,10 +1002,10 @@
         <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>27</v>
@@ -1008,22 +1014,22 @@
         <v>2</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="R2" s="9">
-        <v>32509</v>
+        <v>89</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>10</v>
@@ -1041,7 +1047,7 @@
         <v>13</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Debtor lookup call finish
</commit_message>
<xml_diff>
--- a/testdata/CBO-Smoke-TestData.xlsx
+++ b/testdata/CBO-Smoke-TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Srividhya\Playwright - discovery handson\CBO - Smoke\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Srividhya\Playwright - discovery handson\CBO - Smoke - Jan 28\CBO_Smoke\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3962DAE9-08B8-474A-9C46-B0268ECDB2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F1A128-30A3-4814-B5B6-2B6B19C31517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -79,9 +79,6 @@
     <t>RETAIL</t>
   </si>
   <si>
-    <t>$getcurrentdate</t>
-  </si>
-  <si>
     <t>CBO_Smoke_1</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>APIdateOfBirth</t>
   </si>
   <si>
-    <t>APIadressType</t>
-  </si>
-  <si>
     <t>APIaddress</t>
   </si>
   <si>
@@ -299,6 +293,12 @@
   </si>
   <si>
     <t>01/01/1989</t>
+  </si>
+  <si>
+    <t>APIaddressType</t>
+  </si>
+  <si>
+    <t>$GetAPIID</t>
   </si>
 </sst>
 </file>
@@ -715,13 +715,13 @@
       <selection activeCell="A12" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -729,9 +729,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>3</v>
@@ -750,191 +750,191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E450987-3812-44CB-89CB-24F32111945A}">
-  <dimension ref="A1:BR8"/>
+  <dimension ref="A1:BQ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="20" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="30.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="24" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="26.42578125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="24.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.85546875" style="2" customWidth="1"/>
-    <col min="26" max="26" width="9.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.5546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="27.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="26.44140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13.109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="10.88671875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="9.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="16.88671875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="16.33203125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="24.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.88671875" style="2" customWidth="1"/>
+    <col min="26" max="26" width="9.33203125" style="2" customWidth="1"/>
     <col min="27" max="27" width="10" style="2" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.28515625" style="2" customWidth="1"/>
-    <col min="31" max="31" width="15.7109375" style="2" customWidth="1"/>
-    <col min="32" max="32" width="16.7109375" style="2" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" style="2" customWidth="1"/>
-    <col min="34" max="34" width="19.85546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="11.44140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.33203125" style="2" customWidth="1"/>
+    <col min="31" max="31" width="15.6640625" style="2" customWidth="1"/>
+    <col min="32" max="32" width="16.6640625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="14.44140625" style="2" customWidth="1"/>
+    <col min="34" max="34" width="19.88671875" style="2" customWidth="1"/>
     <col min="35" max="35" width="8" style="2" customWidth="1"/>
-    <col min="36" max="36" width="9.7109375" style="2" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.140625" style="2" customWidth="1"/>
-    <col min="39" max="39" width="8.85546875" style="2"/>
-    <col min="40" max="41" width="15" style="2" customWidth="1"/>
-    <col min="42" max="42" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14" style="2" customWidth="1"/>
-    <col min="44" max="44" width="13.140625" style="2" customWidth="1"/>
-    <col min="45" max="45" width="10.85546875" style="2" customWidth="1"/>
-    <col min="46" max="46" width="8.85546875" style="2"/>
-    <col min="47" max="47" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="8.5703125" style="2" customWidth="1"/>
-    <col min="50" max="50" width="19.42578125" style="2" customWidth="1"/>
-    <col min="51" max="51" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="63" width="8.85546875" style="2"/>
-    <col min="64" max="64" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="65" max="16384" width="8.85546875" style="2"/>
+    <col min="36" max="36" width="9.6640625" style="2" customWidth="1"/>
+    <col min="37" max="37" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.109375" style="2" customWidth="1"/>
+    <col min="39" max="39" width="8.88671875" style="2"/>
+    <col min="40" max="40" width="15" style="2" customWidth="1"/>
+    <col min="41" max="41" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" style="2" customWidth="1"/>
+    <col min="43" max="43" width="13.109375" style="2" customWidth="1"/>
+    <col min="44" max="44" width="10.88671875" style="2" customWidth="1"/>
+    <col min="45" max="45" width="8.88671875" style="2"/>
+    <col min="46" max="46" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.5546875" style="2" customWidth="1"/>
+    <col min="49" max="49" width="19.44140625" style="2" customWidth="1"/>
+    <col min="50" max="50" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="62" width="8.88671875" style="2"/>
+    <col min="63" max="63" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="64" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:69" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="AD1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="AG1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>36</v>
@@ -943,93 +943,90 @@
         <v>37</v>
       </c>
       <c r="AQ1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L2" s="1">
         <v>2</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="R2" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>90</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>10</v>
@@ -1047,7 +1044,7 @@
         <v>13</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>6</v>
@@ -1056,7 +1053,7 @@
         <v>7</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AB2" s="1">
         <v>1005</v>
@@ -1065,7 +1062,7 @@
         <v>8</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>4</v>
@@ -1074,7 +1071,7 @@
         <v>5</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AH2" s="4" t="s">
         <v>6</v>
@@ -1083,7 +1080,7 @@
         <v>7</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AK2" s="1"/>
       <c r="AL2" s="1" t="s">
@@ -1093,58 +1090,55 @@
         <v>2005</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AO2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AP2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ2" s="9">
-        <v>32509</v>
-      </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AP2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AU2" s="5" t="s">
+      <c r="AT2" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="AU2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="AV2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AX2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BA2" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="BC2" s="6"/>
       <c r="BD2" s="6"/>
-      <c r="BE2" s="6"/>
-      <c r="BP2" s="6"/>
-      <c r="BR2" s="7"/>
+      <c r="BO2" s="6"/>
+      <c r="BQ2" s="7"/>
     </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:69" x14ac:dyDescent="0.3">
       <c r="AL5" s="8"/>
-      <c r="AW5" s="8"/>
-      <c r="AY5" s="8"/>
+      <c r="AV5" s="8"/>
+      <c r="AX5" s="8"/>
     </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" x14ac:dyDescent="0.3">
       <c r="AD8" s="8"/>
     </row>
   </sheetData>

</xml_diff>